<commit_message>
adding 12-pole connector to design and BOM
</commit_message>
<xml_diff>
--- a/prj/hazelnut_large/LHC-001/1-Documentation/Large Hazelnut Light Assembly BOM.xlsx
+++ b/prj/hazelnut_large/LHC-001/1-Documentation/Large Hazelnut Light Assembly BOM.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsavas/Documents/git/openag-mechanical/prj/hazelnut_large/LHC-001/1-Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tim\Documents\GitHub\openag-mechanical\prj\hazelnut_large\LHC-001\1-Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3051CD86-E79B-B848-A4CE-51F3955F3F3F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="105">
   <si>
     <t>Description</t>
   </si>
@@ -323,17 +322,29 @@
   </si>
   <si>
     <t>TOTAL COST:</t>
+  </si>
+  <si>
+    <t>12-pole plug</t>
+  </si>
+  <si>
+    <t>3216K670_HARSH ENVIRONMENT MINI CONNECTOR</t>
+  </si>
+  <si>
+    <t>McMaster Carr</t>
+  </si>
+  <si>
+    <t>3216K670</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="###0"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -388,6 +399,12 @@
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -418,10 +435,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -478,10 +496,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -793,42 +814,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:X31"/>
+  <dimension ref="A1:X32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U22" sqref="U22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.83203125" customWidth="1"/>
-    <col min="2" max="2" width="18.83203125" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" customWidth="1"/>
-    <col min="6" max="6" width="17.5" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5" customWidth="1"/>
-    <col min="9" max="9" width="16.5" customWidth="1"/>
-    <col min="10" max="10" width="22.83203125" customWidth="1"/>
-    <col min="11" max="11" width="14.5" customWidth="1"/>
-    <col min="12" max="12" width="19.6640625" customWidth="1"/>
-    <col min="13" max="13" width="13.83203125" customWidth="1"/>
+    <col min="1" max="1" width="47.81640625" customWidth="1"/>
+    <col min="2" max="2" width="18.81640625" customWidth="1"/>
+    <col min="3" max="3" width="16.81640625" customWidth="1"/>
+    <col min="4" max="4" width="14.6328125" customWidth="1"/>
+    <col min="5" max="5" width="17.36328125" customWidth="1"/>
+    <col min="6" max="6" width="17.453125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="19.36328125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="14.453125" customWidth="1"/>
+    <col min="9" max="9" width="16.453125" customWidth="1"/>
+    <col min="10" max="10" width="22.81640625" customWidth="1"/>
+    <col min="11" max="11" width="14.453125" customWidth="1"/>
+    <col min="12" max="12" width="19.6328125" customWidth="1"/>
+    <col min="13" max="13" width="13.81640625" customWidth="1"/>
     <col min="14" max="15" width="18" customWidth="1"/>
-    <col min="16" max="16" width="19.6640625" customWidth="1"/>
-    <col min="17" max="18" width="14.5" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="22.5" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="18.33203125" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="14.5" customWidth="1"/>
-    <col min="22" max="24" width="15.83203125" hidden="1"/>
-    <col min="25" max="16384" width="14.5" hidden="1"/>
+    <col min="16" max="16" width="19.6328125" customWidth="1"/>
+    <col min="17" max="18" width="14.453125" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="22.453125" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="18.36328125" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="14.453125" customWidth="1"/>
+    <col min="22" max="24" width="15.81640625" hidden="1" customWidth="1"/>
+    <col min="25" max="16384" width="14.453125" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -902,7 +924,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -968,7 +990,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>29</v>
       </c>
@@ -1028,7 +1050,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>34</v>
       </c>
@@ -1088,7 +1110,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>40</v>
       </c>
@@ -1135,7 +1157,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>45</v>
       </c>
@@ -1182,7 +1204,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>48</v>
       </c>
@@ -1229,7 +1251,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>54</v>
       </c>
@@ -1277,7 +1299,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>58</v>
       </c>
@@ -1324,7 +1346,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>61</v>
       </c>
@@ -1368,7 +1390,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>63</v>
       </c>
@@ -1412,7 +1434,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>65</v>
       </c>
@@ -1456,7 +1478,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>67</v>
       </c>
@@ -1500,7 +1522,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>69</v>
       </c>
@@ -1544,7 +1566,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>71</v>
       </c>
@@ -1588,7 +1610,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>73</v>
       </c>
@@ -1612,7 +1634,7 @@
       <c r="N16" s="22"/>
       <c r="O16" s="22"/>
     </row>
-    <row r="17" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>75</v>
       </c>
@@ -1656,7 +1678,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>77</v>
       </c>
@@ -1711,7 +1733,7 @@
       <c r="W18" s="26"/>
       <c r="X18" s="26"/>
     </row>
-    <row r="19" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>79</v>
       </c>
@@ -1758,7 +1780,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>82</v>
       </c>
@@ -1802,7 +1824,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>85</v>
       </c>
@@ -1817,7 +1839,7 @@
       <c r="N21" s="22"/>
       <c r="O21" s="22"/>
     </row>
-    <row r="22" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>86</v>
       </c>
@@ -1832,91 +1854,94 @@
       <c r="N22" s="22"/>
       <c r="O22" s="22"/>
     </row>
-    <row r="23" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="2" t="s">
+    <row r="23" spans="1:24" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="36">
+        <v>1</v>
+      </c>
+      <c r="E23" s="14">
+        <f t="shared" ref="E23" si="3">D23*50</f>
+        <v>50</v>
+      </c>
+      <c r="H23" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="I23" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="J23" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="K23" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="L23" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="M23" s="21">
+        <v>98.16</v>
+      </c>
+      <c r="N23" s="17">
+        <f t="shared" ref="N23" si="4">M23*E23</f>
+        <v>4908</v>
+      </c>
+      <c r="O23" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="P23" s="22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B24" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D24" s="2">
         <v>1</v>
       </c>
-      <c r="E23" s="4">
-        <f t="shared" ref="E23:E27" si="3">D23*50</f>
+      <c r="E24" s="4">
+        <f t="shared" ref="E24:E28" si="5">D24*50</f>
         <v>50</v>
       </c>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="2" t="s">
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="J23" s="2" t="s">
+      <c r="J24" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="K23" s="10" t="str">
+      <c r="K24" s="10" t="str">
         <f>HYPERLINK("https://www.fleximounts.com/product-category/monitor-mounts/?filtering=1&amp;filter_display-type=single-display","Fleximount")</f>
         <v>Fleximount</v>
       </c>
-      <c r="L23" s="9"/>
-      <c r="M23" s="6">
+      <c r="L24" s="9"/>
+      <c r="M24" s="6">
         <v>49.99</v>
       </c>
-      <c r="N23" s="6">
-        <f>M23*E23</f>
+      <c r="N24" s="6">
+        <f>M24*E24</f>
         <v>2499.5</v>
       </c>
-      <c r="O23" s="31"/>
-      <c r="P23" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q23" s="9"/>
-      <c r="R23" s="9"/>
-      <c r="S23" s="9"/>
-      <c r="T23" s="9"/>
-      <c r="U23" s="9"/>
-      <c r="V23" s="9"/>
-      <c r="W23" s="9"/>
-      <c r="X23" s="9"/>
-    </row>
-    <row r="24" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="2">
-        <v>1</v>
-      </c>
-      <c r="E24" s="4">
-        <f t="shared" si="3"/>
-        <v>50</v>
-      </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="32"/>
-      <c r="N24" s="31"/>
       <c r="O24" s="31"/>
-      <c r="P24" s="9"/>
+      <c r="P24" s="8" t="s">
+        <v>53</v>
+      </c>
       <c r="Q24" s="9"/>
       <c r="R24" s="9"/>
       <c r="S24" s="9"/>
@@ -1926,9 +1951,9 @@
       <c r="W24" s="9"/>
       <c r="X24" s="9"/>
     </row>
-    <row r="25" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>91</v>
@@ -1937,16 +1962,16 @@
         <v>35</v>
       </c>
       <c r="D25" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E25" s="4">
-        <f t="shared" si="3"/>
-        <v>100</v>
+        <f t="shared" si="5"/>
+        <v>50</v>
       </c>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
       <c r="H25" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>93</v>
@@ -1969,9 +1994,9 @@
       <c r="W25" s="9"/>
       <c r="X25" s="9"/>
     </row>
-    <row r="26" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>91</v>
@@ -1980,15 +2005,17 @@
         <v>35</v>
       </c>
       <c r="D26" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E26" s="4">
-        <f t="shared" si="3"/>
-        <v>50</v>
+        <f t="shared" si="5"/>
+        <v>100</v>
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
+      <c r="H26" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="I26" s="2" t="s">
         <v>93</v>
       </c>
@@ -2010,28 +2037,32 @@
       <c r="W26" s="9"/>
       <c r="X26" s="9"/>
     </row>
-    <row r="27" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>22</v>
+        <v>91</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D27" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E27" s="4">
-        <f t="shared" si="3"/>
-        <v>100</v>
+        <f t="shared" si="5"/>
+        <v>50</v>
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
+      <c r="I27" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="K27" s="9"/>
       <c r="L27" s="9"/>
       <c r="M27" s="32"/>
@@ -2047,36 +2078,47 @@
       <c r="W27" s="9"/>
       <c r="X27" s="9"/>
     </row>
-    <row r="28" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="23" t="s">
+    <row r="28" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="2">
+        <v>2</v>
+      </c>
+      <c r="E28" s="4">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="32"/>
+      <c r="N28" s="31"/>
+      <c r="O28" s="31"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9"/>
+      <c r="S28" s="9"/>
+      <c r="T28" s="9"/>
+      <c r="U28" s="9"/>
+      <c r="V28" s="9"/>
+      <c r="W28" s="9"/>
+      <c r="X28" s="9"/>
+    </row>
+    <row r="29" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="26"/>
-      <c r="M28" s="33"/>
-      <c r="N28" s="34"/>
-      <c r="O28" s="34"/>
-      <c r="P28" s="26"/>
-      <c r="Q28" s="26"/>
-      <c r="R28" s="26"/>
-      <c r="S28" s="26"/>
-      <c r="T28" s="26"/>
-      <c r="U28" s="26"/>
-      <c r="V28" s="26"/>
-      <c r="W28" s="26"/>
-      <c r="X28" s="26"/>
-    </row>
-    <row r="29" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="23"/>
       <c r="B29" s="24"/>
       <c r="C29" s="24"/>
       <c r="D29" s="23"/>
@@ -2101,29 +2143,21 @@
       <c r="W29" s="26"/>
       <c r="X29" s="26"/>
     </row>
-    <row r="30" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="36" t="s">
-        <v>100</v>
-      </c>
-      <c r="B30" s="37"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="37"/>
-      <c r="H30" s="37"/>
-      <c r="I30" s="37"/>
-      <c r="J30" s="37"/>
-      <c r="K30" s="37"/>
-      <c r="L30" s="37"/>
-      <c r="M30" s="33">
-        <f t="shared" ref="M30:N30" si="4">SUM(M2:M27)</f>
-        <v>667.54</v>
-      </c>
-      <c r="N30" s="35">
-        <f t="shared" si="4"/>
-        <v>40922.58833333334</v>
-      </c>
+    <row r="30" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="23"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="23"/>
+      <c r="K30" s="26"/>
+      <c r="L30" s="26"/>
+      <c r="M30" s="33"/>
+      <c r="N30" s="34"/>
       <c r="O30" s="34"/>
       <c r="P30" s="26"/>
       <c r="Q30" s="26"/>
@@ -2135,19 +2169,56 @@
       <c r="W30" s="26"/>
       <c r="X30" s="26"/>
     </row>
-    <row r="31" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="31" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="38"/>
+      <c r="K31" s="38"/>
+      <c r="L31" s="38"/>
+      <c r="M31" s="33">
+        <f t="shared" ref="M31:N31" si="6">SUM(M2:M28)</f>
+        <v>765.69999999999993</v>
+      </c>
+      <c r="N31" s="35">
+        <f t="shared" si="6"/>
+        <v>45830.58833333334</v>
+      </c>
+      <c r="O31" s="34"/>
+      <c r="P31" s="26"/>
+      <c r="Q31" s="26"/>
+      <c r="R31" s="26"/>
+      <c r="S31" s="26"/>
+      <c r="T31" s="26"/>
+      <c r="U31" s="26"/>
+      <c r="V31" s="26"/>
+      <c r="W31" s="26"/>
+      <c r="X31" s="26"/>
+    </row>
+    <row r="32" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A30:L30"/>
+    <mergeCell ref="A31:L31"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="C2:C29" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="C2:C30">
       <formula1>"In Design,In Testing,Validated"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="B2:B29" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" sqref="B2:B30">
       <formula1>"Stock Part,Stock Material,Custom Part,Other"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="K23" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding mounting bracket to lrg hz light and bom changes
</commit_message>
<xml_diff>
--- a/prj/hazelnut_large/LHC-001/1-Documentation/Large Hazelnut Light Assembly BOM.xlsx
+++ b/prj/hazelnut_large/LHC-001/1-Documentation/Large Hazelnut Light Assembly BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="107">
   <si>
     <t>Description</t>
   </si>
@@ -334,6 +334,12 @@
   </si>
   <si>
     <t>3216K670</t>
+  </si>
+  <si>
+    <t>Delrin or metal mounting bracket, back of enclosure</t>
+  </si>
+  <si>
+    <t>Quantity for 10 Assemblies</t>
   </si>
 </sst>
 </file>
@@ -439,7 +445,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -497,9 +503,11 @@
     </xf>
     <xf numFmtId="165" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -818,11 +826,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:X32"/>
+  <dimension ref="A1:Y32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U22" sqref="U22"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -831,26 +839,27 @@
     <col min="2" max="2" width="18.81640625" customWidth="1"/>
     <col min="3" max="3" width="16.81640625" customWidth="1"/>
     <col min="4" max="4" width="14.6328125" customWidth="1"/>
-    <col min="5" max="5" width="17.36328125" customWidth="1"/>
-    <col min="6" max="6" width="17.453125" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="19.36328125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="14.453125" customWidth="1"/>
-    <col min="9" max="9" width="16.453125" customWidth="1"/>
-    <col min="10" max="10" width="22.81640625" customWidth="1"/>
-    <col min="11" max="11" width="14.453125" customWidth="1"/>
-    <col min="12" max="12" width="19.6328125" customWidth="1"/>
-    <col min="13" max="13" width="13.81640625" customWidth="1"/>
-    <col min="14" max="15" width="18" customWidth="1"/>
-    <col min="16" max="16" width="19.6328125" customWidth="1"/>
-    <col min="17" max="18" width="14.453125" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="22.453125" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="18.36328125" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="14.453125" customWidth="1"/>
-    <col min="22" max="24" width="15.81640625" hidden="1" customWidth="1"/>
-    <col min="25" max="16384" width="14.453125" hidden="1"/>
+    <col min="5" max="5" width="14.6328125" style="37" customWidth="1"/>
+    <col min="6" max="6" width="17.36328125" customWidth="1"/>
+    <col min="7" max="7" width="17.453125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="19.36328125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" customWidth="1"/>
+    <col min="10" max="10" width="16.453125" customWidth="1"/>
+    <col min="11" max="11" width="22.81640625" customWidth="1"/>
+    <col min="12" max="12" width="14.453125" customWidth="1"/>
+    <col min="13" max="13" width="19.6328125" customWidth="1"/>
+    <col min="14" max="14" width="13.81640625" customWidth="1"/>
+    <col min="15" max="16" width="18" customWidth="1"/>
+    <col min="17" max="17" width="19.6328125" customWidth="1"/>
+    <col min="18" max="19" width="14.453125" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="22.453125" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="18.36328125" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="14.453125" customWidth="1"/>
+    <col min="23" max="25" width="15.81640625" hidden="1" customWidth="1"/>
+    <col min="26" max="16384" width="14.453125" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -864,67 +873,70 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -937,60 +949,64 @@
       <c r="D2" s="3">
         <v>6</v>
       </c>
-      <c r="E2" s="4">
-        <f t="shared" ref="E2:E20" si="0">D2*50</f>
+      <c r="E2" s="3">
+        <f>D2*10</f>
+        <v>60</v>
+      </c>
+      <c r="F2" s="4">
+        <f t="shared" ref="F2:F20" si="0">D2*50</f>
         <v>300</v>
       </c>
-      <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="3"/>
+      <c r="I2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="5" t="str">
+      <c r="L2" s="5" t="str">
         <f>HYPERLINK("https://www.digikey.com/products/en?keywords=PL1825SR%E2%80%8E","Digikey")</f>
         <v>Digikey</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="6">
+      <c r="N2" s="6">
         <v>17.97</v>
       </c>
-      <c r="N2" s="7">
-        <f t="shared" ref="N2:N15" si="1">M2*E2</f>
+      <c r="O2" s="7">
+        <f t="shared" ref="O2:O15" si="1">N2*F2</f>
         <v>5391</v>
       </c>
-      <c r="O2" s="8">
+      <c r="P2" s="8">
         <v>16</v>
       </c>
-      <c r="P2" s="2">
+      <c r="Q2" s="2">
         <v>8</v>
       </c>
-      <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
-      <c r="S2" s="9"/>
+      <c r="S2" s="2"/>
       <c r="T2" s="9"/>
-      <c r="U2" s="10" t="str">
+      <c r="U2" s="9"/>
+      <c r="V2" s="10" t="str">
         <f>HYPERLINK("http://www.khatod.com/product.php?product=3758","Khatod")</f>
         <v>Khatod</v>
       </c>
-      <c r="V2" s="11" t="s">
-        <v>28</v>
-      </c>
       <c r="W2" s="11" t="s">
         <v>28</v>
       </c>
       <c r="X2" s="11" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y2" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>29</v>
       </c>
@@ -1003,54 +1019,58 @@
       <c r="D3" s="12">
         <v>1</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="41">
+        <f t="shared" ref="E3:E28" si="2">D3*10</f>
+        <v>10</v>
+      </c>
+      <c r="F3" s="14">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="I3" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="J3" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="K3" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="15" t="str">
+      <c r="L3" s="15" t="str">
         <f>HYPERLINK("https://www.digikey.com/product-detail/en/aavid-thermal-division-of-boyd-corporation/416201U00000G/416201U00000G-ND/6131504","Digikey")</f>
         <v>Digikey</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="M3" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="M3" s="16">
+      <c r="N3" s="16">
         <v>105.3</v>
       </c>
-      <c r="N3" s="17">
+      <c r="O3" s="17">
         <f t="shared" si="1"/>
         <v>5265</v>
       </c>
-      <c r="O3" s="18">
+      <c r="P3" s="18">
         <v>92</v>
       </c>
-      <c r="P3" s="12">
+      <c r="Q3" s="12">
         <v>8</v>
       </c>
-      <c r="U3" s="19" t="str">
+      <c r="V3" s="19" t="str">
         <f>HYPERLINK("https://www.mouser.com/ProductDetail/Aavid/416201U00000G?qs=Kvtkb%2Foz0wd%252b2DwBgC9QwQ%3D%3D&amp;gclid=Cj0KCQjwsZ3kBRCnARIsAIuAV_SCzW8MMEduJokoG7mhrmGWY7vjMiJKFcZbTnGTYMEb1N04ey1WXucaAhcLEALw_wcB","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="V3" s="16">
+      <c r="W3" s="16">
         <v>80.73</v>
       </c>
-      <c r="W3" s="12">
+      <c r="X3" s="12">
         <v>59</v>
       </c>
-      <c r="X3" s="12">
+      <c r="Y3" s="12">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>34</v>
       </c>
@@ -1063,54 +1083,58 @@
       <c r="D4" s="12">
         <v>6</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="41">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="F4" s="14">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="I4" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="J4" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="K4" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="K4" s="15" t="str">
+      <c r="L4" s="15" t="str">
         <f>HYPERLINK("https://www.digikey.com/product-detail/en/erp-power-llc/SLM160W-3.9-40-ZA/1800-1101-ND/7496304","Digikey")</f>
         <v>Digikey</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="M4" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="M4" s="16">
+      <c r="N4" s="16">
         <v>57.71</v>
       </c>
-      <c r="N4" s="17">
+      <c r="O4" s="17">
         <f t="shared" si="1"/>
         <v>17313</v>
       </c>
-      <c r="O4" s="18">
+      <c r="P4" s="18">
         <v>9</v>
       </c>
-      <c r="P4" s="12">
+      <c r="Q4" s="12">
         <v>6</v>
       </c>
-      <c r="U4" s="19" t="str">
+      <c r="V4" s="19" t="str">
         <f>HYPERLINK("https://www.mouser.com/ProductDetail/ERP/SLM160W-39-40-ZA?qs=Ey4jopcCj2pGCn1F%2FZnO1g%3D%3D","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="V4" s="16">
+      <c r="W4" s="16">
         <v>50.09</v>
       </c>
-      <c r="W4" s="12">
+      <c r="X4" s="12">
         <v>50</v>
       </c>
-      <c r="X4" s="12">
+      <c r="Y4" s="12">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>40</v>
       </c>
@@ -1123,41 +1147,45 @@
       <c r="D5" s="12">
         <v>2</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="41">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="F5" s="14">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="I5" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="J5" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="K5" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="K5" s="15" t="str">
+      <c r="L5" s="15" t="str">
         <f>HYPERLINK("https://www.digikey.com/product-detail/en/bridgelux/BXRC-50C10K1-D-74-SE/976-1596-ND/6557098","Digikey")</f>
         <v>Digikey</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="M5" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="M5" s="16">
+      <c r="N5" s="16">
         <v>22.98</v>
       </c>
-      <c r="N5" s="17">
+      <c r="O5" s="17">
         <f t="shared" si="1"/>
         <v>2298</v>
       </c>
-      <c r="O5" s="18">
+      <c r="P5" s="18">
         <v>1699</v>
       </c>
-      <c r="P5" s="12">
+      <c r="Q5" s="12">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>45</v>
       </c>
@@ -1170,41 +1198,45 @@
       <c r="D6" s="12">
         <v>2</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="41">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="F6" s="14">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="I6" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="J6" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="K6" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="K6" s="15" t="str">
+      <c r="L6" s="15" t="str">
         <f>HYPERLINK("https://www.digikey.com/product-detail/en/bridgelux/BXRC-30E10K0-D-73-SE/976-1590-ND/6557092","Digikey")</f>
         <v>Digikey</v>
       </c>
-      <c r="L6" s="12" t="s">
+      <c r="M6" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="M6" s="16">
+      <c r="N6" s="16">
         <v>22.98</v>
       </c>
-      <c r="N6" s="17">
+      <c r="O6" s="17">
         <f t="shared" si="1"/>
         <v>2298</v>
       </c>
-      <c r="O6" s="18">
+      <c r="P6" s="18">
         <v>423</v>
       </c>
-      <c r="P6" s="12">
+      <c r="Q6" s="12">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>48</v>
       </c>
@@ -1217,41 +1249,45 @@
       <c r="D7" s="12">
         <v>1</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="41">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="F7" s="14">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="I7" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="I7" s="12" t="s">
-        <v>51</v>
-      </c>
       <c r="J7" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="K7" s="15" t="str">
+      <c r="K7" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L7" s="15" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/1376n13","McMaster Carr")</f>
         <v>McMaster Carr</v>
       </c>
-      <c r="L7" s="12" t="s">
+      <c r="M7" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="M7" s="16">
+      <c r="N7" s="16">
         <v>10.38</v>
       </c>
-      <c r="N7" s="17">
+      <c r="O7" s="17">
         <f t="shared" si="1"/>
         <v>519</v>
       </c>
-      <c r="O7" s="18" t="s">
-        <v>53</v>
-      </c>
       <c r="P7" s="18" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q7" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>54</v>
       </c>
@@ -1265,41 +1301,45 @@
         <f>1/15</f>
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="41">
+        <f t="shared" si="2"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F8" s="14">
         <f t="shared" si="0"/>
         <v>3.3333333333333335</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="I8" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="I8" s="12" t="s">
-        <v>51</v>
-      </c>
       <c r="J8" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="K8" s="15" t="str">
+      <c r="K8" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L8" s="15" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/89015k59","McMaster Carr")</f>
         <v>McMaster Carr</v>
       </c>
-      <c r="L8" s="12" t="s">
+      <c r="M8" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="M8" s="16">
+      <c r="N8" s="16">
         <v>191.8</v>
       </c>
-      <c r="N8" s="17">
+      <c r="O8" s="17">
         <f t="shared" si="1"/>
         <v>639.33333333333337</v>
       </c>
-      <c r="O8" s="18" t="s">
-        <v>53</v>
-      </c>
       <c r="P8" s="18" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q8" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>58</v>
       </c>
@@ -1312,41 +1352,45 @@
       <c r="D9" s="20">
         <v>0.05</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="41">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="F9" s="14">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="I9" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="I9" s="12" t="s">
-        <v>51</v>
-      </c>
       <c r="J9" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="K9" s="15" t="str">
+      <c r="K9" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L9" s="15" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/8505k753","McMaster Carr")</f>
         <v>McMaster Carr</v>
       </c>
-      <c r="L9" s="12" t="s">
+      <c r="M9" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="M9" s="16">
+      <c r="N9" s="16">
         <v>99.41</v>
       </c>
-      <c r="N9" s="17">
+      <c r="O9" s="17">
         <f t="shared" si="1"/>
         <v>248.52499999999998</v>
       </c>
-      <c r="O9" s="18" t="s">
-        <v>53</v>
-      </c>
       <c r="P9" s="18" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q9" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>61</v>
       </c>
@@ -1359,38 +1403,42 @@
       <c r="D10" s="12">
         <v>0.12</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="41">
+        <f t="shared" si="2"/>
+        <v>1.2</v>
+      </c>
+      <c r="F10" s="14">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="I10" s="12" t="s">
-        <v>51</v>
-      </c>
       <c r="J10" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="K10" s="15" t="str">
+      <c r="K10" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L10" s="15" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/91773a103","McMaster Carr")</f>
         <v>McMaster Carr</v>
       </c>
-      <c r="L10" s="12" t="s">
+      <c r="M10" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="M10" s="16">
+      <c r="N10" s="16">
         <v>8.26</v>
       </c>
-      <c r="N10" s="17">
+      <c r="O10" s="17">
         <f t="shared" si="1"/>
         <v>49.56</v>
       </c>
-      <c r="O10" s="18" t="s">
-        <v>53</v>
-      </c>
       <c r="P10" s="18" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q10" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>63</v>
       </c>
@@ -1403,38 +1451,42 @@
       <c r="D11" s="12">
         <v>0.04</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="41">
+        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
+      <c r="F11" s="14">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="I11" s="12" t="s">
-        <v>51</v>
-      </c>
       <c r="J11" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="K11" s="15" t="str">
+      <c r="K11" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L11" s="15" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/92949a152","McMaster Carr")</f>
         <v>McMaster Carr</v>
       </c>
-      <c r="L11" s="12" t="s">
+      <c r="M11" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="M11" s="16">
+      <c r="N11" s="16">
         <v>6.22</v>
       </c>
-      <c r="N11" s="17">
+      <c r="O11" s="17">
         <f t="shared" si="1"/>
         <v>12.44</v>
       </c>
-      <c r="O11" s="18" t="s">
-        <v>53</v>
-      </c>
       <c r="P11" s="18" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q11" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>65</v>
       </c>
@@ -1447,38 +1499,42 @@
       <c r="D12" s="12">
         <v>0.04</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="41">
+        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
+      <c r="F12" s="14">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="I12" s="13" t="s">
-        <v>51</v>
-      </c>
       <c r="J12" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="K12" s="15" t="str">
+      <c r="K12" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="L12" s="15" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/90257a007","McMaster Carr")</f>
         <v>McMaster Carr</v>
       </c>
-      <c r="L12" s="12" t="s">
+      <c r="M12" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="M12" s="16">
+      <c r="N12" s="16">
         <v>6.75</v>
       </c>
-      <c r="N12" s="17">
+      <c r="O12" s="17">
         <f t="shared" si="1"/>
         <v>13.5</v>
       </c>
-      <c r="O12" s="18" t="s">
-        <v>53</v>
-      </c>
       <c r="P12" s="18" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q12" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>67</v>
       </c>
@@ -1491,38 +1547,42 @@
       <c r="D13" s="12">
         <v>0.04</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="41">
+        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
+      <c r="F13" s="14">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="I13" s="13" t="s">
-        <v>51</v>
-      </c>
       <c r="J13" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="K13" s="15" t="str">
+      <c r="K13" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="L13" s="15" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/90127a007","McMaster Carr")</f>
         <v>McMaster Carr</v>
       </c>
-      <c r="L13" s="12" t="s">
+      <c r="M13" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="M13" s="16">
+      <c r="N13" s="16">
         <v>8.5</v>
       </c>
-      <c r="N13" s="17">
+      <c r="O13" s="17">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="O13" s="18" t="s">
-        <v>53</v>
-      </c>
       <c r="P13" s="18" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q13" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>69</v>
       </c>
@@ -1535,38 +1595,42 @@
       <c r="D14" s="12">
         <v>0.1</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="41">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F14" s="14">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="I14" s="12" t="s">
-        <v>51</v>
-      </c>
       <c r="J14" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="K14" s="15" t="str">
+      <c r="K14" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L14" s="15" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/92949a198","McMaster Carr")</f>
         <v>McMaster Carr</v>
       </c>
-      <c r="L14" s="12" t="s">
+      <c r="M14" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="M14" s="16">
+      <c r="N14" s="16">
         <v>8.09</v>
       </c>
-      <c r="N14" s="17">
+      <c r="O14" s="17">
         <f t="shared" si="1"/>
         <v>40.450000000000003</v>
       </c>
-      <c r="O14" s="18" t="s">
-        <v>53</v>
-      </c>
       <c r="P14" s="18" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q14" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>71</v>
       </c>
@@ -1579,38 +1643,42 @@
       <c r="D15" s="12">
         <v>0.2</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="41">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="F15" s="14">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="I15" s="12" t="s">
-        <v>51</v>
-      </c>
       <c r="J15" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="K15" s="15" t="str">
+      <c r="K15" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L15" s="15" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/93886a120","McMaster Carr")</f>
         <v>McMaster Carr</v>
       </c>
-      <c r="L15" s="12" t="s">
+      <c r="M15" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="M15" s="16">
+      <c r="N15" s="16">
         <v>8.0299999999999994</v>
       </c>
-      <c r="N15" s="17">
+      <c r="O15" s="17">
         <f t="shared" si="1"/>
         <v>80.3</v>
       </c>
-      <c r="O15" s="18" t="s">
-        <v>53</v>
-      </c>
       <c r="P15" s="18" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q15" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>73</v>
       </c>
@@ -1623,18 +1691,22 @@
       <c r="D16" s="12">
         <v>2</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="41">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="F16" s="14">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="H16" s="12" t="s">
+      <c r="I16" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="M16" s="21"/>
-      <c r="N16" s="22"/>
+      <c r="N16" s="21"/>
       <c r="O16" s="22"/>
-    </row>
-    <row r="17" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P16" s="22"/>
+    </row>
+    <row r="17" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>75</v>
       </c>
@@ -1647,38 +1719,42 @@
       <c r="D17" s="12">
         <v>2</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="41">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="F17" s="14">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="I17" s="12" t="s">
-        <v>51</v>
-      </c>
       <c r="J17" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="K17" s="15" t="str">
+      <c r="K17" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L17" s="15" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/51545k73","McMaster Carr")</f>
         <v>McMaster Carr</v>
       </c>
-      <c r="L17" s="12" t="s">
+      <c r="M17" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="M17" s="16">
+      <c r="N17" s="16">
         <v>18.63</v>
       </c>
-      <c r="N17" s="17">
-        <f t="shared" ref="N17:N20" si="2">M17*E17</f>
+      <c r="O17" s="17">
+        <f t="shared" ref="O17:O20" si="3">N17*F17</f>
         <v>1863</v>
       </c>
-      <c r="O17" s="18" t="s">
-        <v>53</v>
-      </c>
       <c r="P17" s="18" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="18" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q17" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>77</v>
       </c>
@@ -1691,40 +1767,43 @@
       <c r="D18" s="23">
         <v>2</v>
       </c>
-      <c r="E18" s="25">
+      <c r="E18" s="41">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="F18" s="25">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="F18" s="26"/>
       <c r="G18" s="26"/>
       <c r="H18" s="26"/>
-      <c r="I18" s="23" t="s">
-        <v>51</v>
-      </c>
+      <c r="I18" s="26"/>
       <c r="J18" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="K18" s="27" t="str">
+      <c r="K18" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="L18" s="27" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/51545k79","McMaster Carr")</f>
         <v>McMaster Carr</v>
       </c>
-      <c r="L18" s="23" t="s">
+      <c r="M18" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="M18" s="28">
+      <c r="N18" s="28">
         <v>13.55</v>
       </c>
-      <c r="N18" s="29">
-        <f t="shared" si="2"/>
+      <c r="O18" s="29">
+        <f t="shared" si="3"/>
         <v>1355</v>
       </c>
-      <c r="O18" s="30" t="s">
-        <v>53</v>
-      </c>
       <c r="P18" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="Q18" s="26"/>
+      <c r="Q18" s="30" t="s">
+        <v>53</v>
+      </c>
       <c r="R18" s="26"/>
       <c r="S18" s="26"/>
       <c r="T18" s="26"/>
@@ -1732,8 +1811,9 @@
       <c r="V18" s="26"/>
       <c r="W18" s="26"/>
       <c r="X18" s="26"/>
-    </row>
-    <row r="19" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y18" s="26"/>
+    </row>
+    <row r="19" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>79</v>
       </c>
@@ -1746,41 +1826,45 @@
       <c r="D19" s="12">
         <v>20</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19" s="41">
+        <f t="shared" si="2"/>
+        <v>200</v>
+      </c>
+      <c r="F19" s="14">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="H19" s="12" t="s">
+      <c r="I19" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="I19" s="12" t="s">
-        <v>51</v>
-      </c>
       <c r="J19" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="K19" s="15" t="str">
+      <c r="K19" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L19" s="15" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/cadinlnord/5648k263","McMaster Carr")</f>
         <v>McMaster Carr</v>
       </c>
-      <c r="L19" s="12" t="s">
+      <c r="M19" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="M19" s="16">
+      <c r="N19" s="16">
         <v>1</v>
       </c>
-      <c r="N19" s="17">
-        <f t="shared" si="2"/>
+      <c r="O19" s="17">
+        <f t="shared" si="3"/>
         <v>1000</v>
       </c>
-      <c r="O19" s="18" t="s">
-        <v>53</v>
-      </c>
       <c r="P19" s="18" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="20" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q19" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>82</v>
       </c>
@@ -1793,38 +1877,42 @@
       <c r="D20" s="12">
         <v>0.04</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="41">
+        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
+      <c r="F20" s="14">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="I20" s="12" t="s">
+      <c r="J20" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="J20" s="12" t="s">
+      <c r="K20" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="K20" s="15" t="str">
+      <c r="L20" s="15" t="str">
         <f>HYPERLINK("https://www.amazon.com/MY-700-50g-Thermal-Compound-Paste-Conductivity/dp/B07H1PGY7X/ref=sr_1_21_sspa?keywords=thermal+paste&amp;qid=1552396651&amp;s=gateway&amp;sr=8-21-spons&amp;psc=1","Amazon")</f>
         <v>Amazon</v>
       </c>
-      <c r="L20" s="12" t="s">
+      <c r="M20" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="M20" s="16">
+      <c r="N20" s="16">
         <v>9.99</v>
       </c>
-      <c r="N20" s="17">
-        <f t="shared" si="2"/>
+      <c r="O20" s="17">
+        <f t="shared" si="3"/>
         <v>19.98</v>
       </c>
-      <c r="O20" s="18" t="s">
-        <v>53</v>
-      </c>
       <c r="P20" s="18" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="21" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q20" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>85</v>
       </c>
@@ -1834,12 +1922,16 @@
       <c r="C21" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="13"/>
-      <c r="M21" s="21"/>
-      <c r="N21" s="22"/>
+      <c r="E21" s="41">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="13"/>
+      <c r="N21" s="21"/>
       <c r="O21" s="22"/>
-    </row>
-    <row r="22" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P21" s="22"/>
+    </row>
+    <row r="22" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>86</v>
       </c>
@@ -1849,12 +1941,16 @@
       <c r="C22" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E22" s="13"/>
-      <c r="M22" s="21"/>
-      <c r="N22" s="22"/>
+      <c r="E22" s="41">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="13"/>
+      <c r="N22" s="21"/>
       <c r="O22" s="22"/>
-    </row>
-    <row r="23" spans="1:24" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P22" s="22"/>
+    </row>
+    <row r="23" spans="1:25" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>101</v>
       </c>
@@ -1867,40 +1963,44 @@
       <c r="D23" s="36">
         <v>1</v>
       </c>
-      <c r="E23" s="14">
-        <f t="shared" ref="E23" si="3">D23*50</f>
+      <c r="E23" s="41">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="F23" s="14">
+        <f t="shared" ref="F23" si="4">D23*50</f>
         <v>50</v>
       </c>
-      <c r="H23" s="36" t="s">
+      <c r="I23" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="I23" s="36" t="s">
-        <v>51</v>
-      </c>
       <c r="J23" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="K23" s="39" t="s">
+      <c r="K23" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="L23" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="L23" s="36" t="s">
+      <c r="M23" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="M23" s="21">
+      <c r="N23" s="21">
         <v>98.16</v>
       </c>
-      <c r="N23" s="17">
-        <f t="shared" ref="N23" si="4">M23*E23</f>
+      <c r="O23" s="17">
+        <f t="shared" ref="O23" si="5">N23*F23</f>
         <v>4908</v>
       </c>
-      <c r="O23" s="22" t="s">
-        <v>53</v>
-      </c>
       <c r="P23" s="22" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="24" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q23" s="22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>87</v>
       </c>
@@ -1913,36 +2013,39 @@
       <c r="D24" s="2">
         <v>1</v>
       </c>
-      <c r="E24" s="4">
-        <f t="shared" ref="E24:E28" si="5">D24*50</f>
+      <c r="E24" s="3">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="F24" s="4">
+        <f t="shared" ref="F24:F28" si="6">D24*50</f>
         <v>50</v>
       </c>
-      <c r="F24" s="9"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
-      <c r="I24" s="2" t="s">
+      <c r="I24" s="9"/>
+      <c r="J24" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="J24" s="2" t="s">
+      <c r="K24" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="K24" s="10" t="str">
+      <c r="L24" s="10" t="str">
         <f>HYPERLINK("https://www.fleximounts.com/product-category/monitor-mounts/?filtering=1&amp;filter_display-type=single-display","Fleximount")</f>
         <v>Fleximount</v>
       </c>
-      <c r="L24" s="9"/>
-      <c r="M24" s="6">
+      <c r="M24" s="9"/>
+      <c r="N24" s="6">
         <v>49.99</v>
       </c>
-      <c r="N24" s="6">
-        <f>M24*E24</f>
+      <c r="O24" s="6">
+        <f>N24*F24</f>
         <v>2499.5</v>
       </c>
-      <c r="O24" s="31"/>
-      <c r="P24" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q24" s="9"/>
+      <c r="P24" s="31"/>
+      <c r="Q24" s="8" t="s">
+        <v>53</v>
+      </c>
       <c r="R24" s="9"/>
       <c r="S24" s="9"/>
       <c r="T24" s="9"/>
@@ -1950,8 +2053,9 @@
       <c r="V24" s="9"/>
       <c r="W24" s="9"/>
       <c r="X24" s="9"/>
-    </row>
-    <row r="25" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y24" s="9"/>
+    </row>
+    <row r="25" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>90</v>
       </c>
@@ -1964,27 +2068,30 @@
       <c r="D25" s="2">
         <v>1</v>
       </c>
-      <c r="E25" s="4">
-        <f t="shared" si="5"/>
+      <c r="E25" s="3">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="F25" s="4">
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
-      <c r="F25" s="9"/>
       <c r="G25" s="9"/>
-      <c r="H25" s="2" t="s">
+      <c r="H25" s="9"/>
+      <c r="I25" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="I25" s="2" t="s">
+      <c r="J25" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="J25" s="2" t="s">
+      <c r="K25" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="K25" s="9"/>
       <c r="L25" s="9"/>
-      <c r="M25" s="32"/>
-      <c r="N25" s="31"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="32"/>
       <c r="O25" s="31"/>
-      <c r="P25" s="9"/>
+      <c r="P25" s="31"/>
       <c r="Q25" s="9"/>
       <c r="R25" s="9"/>
       <c r="S25" s="9"/>
@@ -1993,8 +2100,9 @@
       <c r="V25" s="9"/>
       <c r="W25" s="9"/>
       <c r="X25" s="9"/>
-    </row>
-    <row r="26" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y25" s="9"/>
+    </row>
+    <row r="26" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>95</v>
       </c>
@@ -2007,27 +2115,30 @@
       <c r="D26" s="2">
         <v>2</v>
       </c>
-      <c r="E26" s="4">
-        <f t="shared" si="5"/>
+      <c r="E26" s="3">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="F26" s="4">
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
-      <c r="F26" s="9"/>
       <c r="G26" s="9"/>
-      <c r="H26" s="2" t="s">
+      <c r="H26" s="9"/>
+      <c r="I26" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="I26" s="2" t="s">
+      <c r="J26" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="J26" s="2" t="s">
+      <c r="K26" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="K26" s="9"/>
       <c r="L26" s="9"/>
-      <c r="M26" s="32"/>
-      <c r="N26" s="31"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="32"/>
       <c r="O26" s="31"/>
-      <c r="P26" s="9"/>
+      <c r="P26" s="31"/>
       <c r="Q26" s="9"/>
       <c r="R26" s="9"/>
       <c r="S26" s="9"/>
@@ -2036,8 +2147,9 @@
       <c r="V26" s="9"/>
       <c r="W26" s="9"/>
       <c r="X26" s="9"/>
-    </row>
-    <row r="27" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y26" s="9"/>
+    </row>
+    <row r="27" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>97</v>
       </c>
@@ -2050,25 +2162,28 @@
       <c r="D27" s="2">
         <v>1</v>
       </c>
-      <c r="E27" s="4">
-        <f t="shared" si="5"/>
+      <c r="E27" s="3">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="F27" s="4">
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
-      <c r="F27" s="9"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
-      <c r="I27" s="2" t="s">
+      <c r="I27" s="9"/>
+      <c r="J27" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="J27" s="2" t="s">
+      <c r="K27" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="K27" s="9"/>
       <c r="L27" s="9"/>
-      <c r="M27" s="32"/>
-      <c r="N27" s="31"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="32"/>
       <c r="O27" s="31"/>
-      <c r="P27" s="9"/>
+      <c r="P27" s="31"/>
       <c r="Q27" s="9"/>
       <c r="R27" s="9"/>
       <c r="S27" s="9"/>
@@ -2077,8 +2192,9 @@
       <c r="V27" s="9"/>
       <c r="W27" s="9"/>
       <c r="X27" s="9"/>
-    </row>
-    <row r="28" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y27" s="9"/>
+    </row>
+    <row r="28" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>98</v>
       </c>
@@ -2091,21 +2207,24 @@
       <c r="D28" s="2">
         <v>2</v>
       </c>
-      <c r="E28" s="4">
-        <f t="shared" si="5"/>
+      <c r="E28" s="3">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="F28" s="4">
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
-      <c r="F28" s="9"/>
       <c r="G28" s="9"/>
       <c r="H28" s="9"/>
       <c r="I28" s="9"/>
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
       <c r="L28" s="9"/>
-      <c r="M28" s="32"/>
-      <c r="N28" s="31"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="32"/>
       <c r="O28" s="31"/>
-      <c r="P28" s="9"/>
+      <c r="P28" s="31"/>
       <c r="Q28" s="9"/>
       <c r="R28" s="9"/>
       <c r="S28" s="9"/>
@@ -2114,26 +2233,27 @@
       <c r="V28" s="9"/>
       <c r="W28" s="9"/>
       <c r="X28" s="9"/>
-    </row>
-    <row r="29" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y28" s="9"/>
+    </row>
+    <row r="29" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="23" t="s">
         <v>99</v>
       </c>
       <c r="B29" s="24"/>
       <c r="C29" s="24"/>
       <c r="D29" s="23"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="26"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="25"/>
       <c r="G29" s="26"/>
       <c r="H29" s="26"/>
-      <c r="I29" s="23"/>
+      <c r="I29" s="26"/>
       <c r="J29" s="23"/>
-      <c r="K29" s="26"/>
+      <c r="K29" s="23"/>
       <c r="L29" s="26"/>
-      <c r="M29" s="33"/>
-      <c r="N29" s="34"/>
+      <c r="M29" s="26"/>
+      <c r="N29" s="33"/>
       <c r="O29" s="34"/>
-      <c r="P29" s="26"/>
+      <c r="P29" s="34"/>
       <c r="Q29" s="26"/>
       <c r="R29" s="26"/>
       <c r="S29" s="26"/>
@@ -2142,24 +2262,36 @@
       <c r="V29" s="26"/>
       <c r="W29" s="26"/>
       <c r="X29" s="26"/>
-    </row>
-    <row r="30" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="23"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="26"/>
+      <c r="Y29" s="26"/>
+    </row>
+    <row r="30" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="B30" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="23">
+        <v>1</v>
+      </c>
+      <c r="E30" s="24"/>
+      <c r="F30" s="14">
+        <f t="shared" ref="F30" si="7">D30*50</f>
+        <v>50</v>
+      </c>
       <c r="G30" s="26"/>
       <c r="H30" s="26"/>
-      <c r="I30" s="23"/>
+      <c r="I30" s="26"/>
       <c r="J30" s="23"/>
-      <c r="K30" s="26"/>
+      <c r="K30" s="23"/>
       <c r="L30" s="26"/>
-      <c r="M30" s="33"/>
-      <c r="N30" s="34"/>
+      <c r="M30" s="26"/>
+      <c r="N30" s="33"/>
       <c r="O30" s="34"/>
-      <c r="P30" s="26"/>
+      <c r="P30" s="34"/>
       <c r="Q30" s="26"/>
       <c r="R30" s="26"/>
       <c r="S30" s="26"/>
@@ -2168,32 +2300,33 @@
       <c r="V30" s="26"/>
       <c r="W30" s="26"/>
       <c r="X30" s="26"/>
-    </row>
-    <row r="31" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="37" t="s">
+      <c r="Y30" s="26"/>
+    </row>
+    <row r="31" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="39" t="s">
         <v>100</v>
       </c>
-      <c r="B31" s="38"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="38"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="38"/>
-      <c r="J31" s="38"/>
-      <c r="K31" s="38"/>
-      <c r="L31" s="38"/>
-      <c r="M31" s="33">
-        <f t="shared" ref="M31:N31" si="6">SUM(M2:M28)</f>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
+      <c r="K31" s="40"/>
+      <c r="L31" s="40"/>
+      <c r="M31" s="40"/>
+      <c r="N31" s="33">
+        <f t="shared" ref="N31:O31" si="8">SUM(N2:N28)</f>
         <v>765.69999999999993</v>
       </c>
-      <c r="N31" s="35">
-        <f t="shared" si="6"/>
+      <c r="O31" s="35">
+        <f t="shared" si="8"/>
         <v>45830.58833333334</v>
       </c>
-      <c r="O31" s="34"/>
-      <c r="P31" s="26"/>
+      <c r="P31" s="34"/>
       <c r="Q31" s="26"/>
       <c r="R31" s="26"/>
       <c r="S31" s="26"/>
@@ -2202,11 +2335,12 @@
       <c r="V31" s="26"/>
       <c r="W31" s="26"/>
       <c r="X31" s="26"/>
-    </row>
-    <row r="32" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="Y31" s="26"/>
+    </row>
+    <row r="32" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A31:L31"/>
+    <mergeCell ref="A31:M31"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" sqref="C2:C30">
@@ -2217,7 +2351,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="K23" r:id="rId1"/>
+    <hyperlink ref="L23" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changed driver line in lrg hz light BOM
</commit_message>
<xml_diff>
--- a/prj/hazelnut_large/LHC-001/1-Documentation/Large Hazelnut Light Assembly BOM.xlsx
+++ b/prj/hazelnut_large/LHC-001/1-Documentation/Large Hazelnut Light Assembly BOM.xlsx
@@ -1,33 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Open AG\Documents\GitHub\openag-mechanical\prj\hazelnut_large\LHC-001\1-Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsavas/Documents/git/openag-mechanical/prj/hazelnut_large/LHC-001/1-Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304CE2A6-962E-4283-B42B-9B22C1AACB48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145E0823-A918-544D-9C8B-E0C989081402}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="107">
   <si>
     <t>Description</t>
   </si>
@@ -320,9 +313,6 @@
     <t>Quantity for 10 Assemblies</t>
   </si>
   <si>
-    <t xml:space="preserve">1866-2579-ND	</t>
-  </si>
-  <si>
     <t>3/16" x 48" x 36" ABS REQUOTE</t>
   </si>
   <si>
@@ -345,6 +335,12 @@
   </si>
   <si>
     <t xml:space="preserve">Mounting arm </t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>1866-2579-ND</t>
   </si>
 </sst>
 </file>
@@ -355,7 +351,7 @@
     <numFmt numFmtId="164" formatCode="###0"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -410,6 +406,12 @@
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -440,10 +442,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -506,8 +509,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -827,37 +832,37 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M19" sqref="M19"/>
+      <selection pane="bottomLeft" activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="47.81640625" customWidth="1"/>
-    <col min="2" max="2" width="18.81640625" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="16.81640625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6328125" customWidth="1"/>
-    <col min="5" max="5" width="14.6328125" style="37" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="17.36328125" customWidth="1"/>
-    <col min="7" max="7" width="17.453125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="19.36328125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="14.453125" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="16.453125" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="22.81640625" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="14.453125" customWidth="1"/>
-    <col min="13" max="13" width="19.6328125" customWidth="1"/>
-    <col min="14" max="14" width="13.81640625" customWidth="1"/>
+    <col min="1" max="1" width="47.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="37" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="17.5" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="22.83203125" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5" customWidth="1"/>
+    <col min="13" max="13" width="19.6640625" customWidth="1"/>
+    <col min="14" max="14" width="13.83203125" customWidth="1"/>
     <col min="15" max="15" width="18" customWidth="1"/>
     <col min="16" max="16" width="18" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="19.6328125" hidden="1" customWidth="1"/>
-    <col min="18" max="19" width="14.453125" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="22.453125" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="18.36328125" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="14.453125" hidden="1" customWidth="1"/>
-    <col min="23" max="25" width="15.81640625" hidden="1" customWidth="1"/>
-    <col min="26" max="16384" width="14.453125" hidden="1"/>
+    <col min="17" max="17" width="19.6640625" hidden="1" customWidth="1"/>
+    <col min="18" max="19" width="14.5" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="22.5" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="18.33203125" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="14.5" hidden="1" customWidth="1"/>
+    <col min="23" max="25" width="15.83203125" hidden="1" customWidth="1"/>
+    <col min="26" max="16384" width="14.5" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -934,7 +939,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -1004,7 +1009,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="12" t="s">
         <v>29</v>
       </c>
@@ -1068,7 +1073,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="12" t="s">
         <v>34</v>
       </c>
@@ -1098,12 +1103,11 @@
       <c r="K4" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="L4" s="15" t="str">
-        <f>HYPERLINK("https://www.digikey.com/product-detail/en/erp-power-llc/SLM160W-3.9-40-ZA/1800-1101-ND/7496304","Digikey")</f>
-        <v>Digikey</v>
+      <c r="L4" s="42" t="s">
+        <v>105</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="N4" s="16">
         <v>169</v>
@@ -1132,7 +1136,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="12" t="s">
         <v>39</v>
       </c>
@@ -1183,7 +1187,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="12" t="s">
         <v>44</v>
       </c>
@@ -1234,7 +1238,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="12" t="s">
         <v>47</v>
       </c>
@@ -1285,7 +1289,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="12" t="s">
         <v>53</v>
       </c>
@@ -1337,9 +1341,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>48</v>
@@ -1388,7 +1392,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="12" t="s">
         <v>59</v>
       </c>
@@ -1436,7 +1440,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="12" t="s">
         <v>61</v>
       </c>
@@ -1484,7 +1488,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="12" t="s">
         <v>63</v>
       </c>
@@ -1532,7 +1536,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="12" t="s">
         <v>65</v>
       </c>
@@ -1580,7 +1584,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="12" t="s">
         <v>67</v>
       </c>
@@ -1628,7 +1632,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="12" t="s">
         <v>69</v>
       </c>
@@ -1676,9 +1680,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>22</v>
@@ -1705,7 +1709,7 @@
         <v>McMaster Carr</v>
       </c>
       <c r="M16" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N16" s="21">
         <v>6.45</v>
@@ -1716,7 +1720,7 @@
       </c>
       <c r="P16" s="22"/>
     </row>
-    <row r="17" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="12" t="s">
         <v>72</v>
       </c>
@@ -1764,7 +1768,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="23" t="s">
         <v>74</v>
       </c>
@@ -1823,9 +1827,9 @@
       <c r="X18" s="26"/>
       <c r="Y18" s="26"/>
     </row>
-    <row r="19" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B19" s="13" t="s">
         <v>22</v>
@@ -1855,7 +1859,7 @@
       </c>
       <c r="L19" s="15"/>
       <c r="M19" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N19" s="16">
         <v>0.28000000000000003</v>
@@ -1871,7 +1875,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="12" t="s">
         <v>77</v>
       </c>
@@ -1919,7 +1923,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="12" t="s">
         <v>80</v>
       </c>
@@ -1938,7 +1942,7 @@
       <c r="O21" s="22"/>
       <c r="P21" s="22"/>
     </row>
-    <row r="22" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="12" t="s">
         <v>81</v>
       </c>
@@ -1957,9 +1961,9 @@
       <c r="O22" s="22"/>
       <c r="P22" s="22"/>
     </row>
-    <row r="23" spans="1:25" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>48</v>
@@ -1992,7 +1996,7 @@
         <v>Digikey</v>
       </c>
       <c r="M23" s="39" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N23" s="21">
         <v>9.1300000000000008</v>
@@ -2008,9 +2012,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>22</v>
@@ -2063,7 +2067,7 @@
       <c r="X24" s="9"/>
       <c r="Y24" s="9"/>
     </row>
-    <row r="25" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
         <v>84</v>
       </c>
@@ -2115,7 +2119,7 @@
       <c r="X25" s="9"/>
       <c r="Y25" s="9"/>
     </row>
-    <row r="26" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
         <v>89</v>
       </c>
@@ -2162,7 +2166,7 @@
       <c r="X26" s="9"/>
       <c r="Y26" s="9"/>
     </row>
-    <row r="27" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
         <v>91</v>
       </c>
@@ -2203,7 +2207,7 @@
       <c r="X27" s="9"/>
       <c r="Y27" s="9"/>
     </row>
-    <row r="28" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="23" t="s">
         <v>92</v>
       </c>
@@ -2232,7 +2236,7 @@
       <c r="X28" s="26"/>
       <c r="Y28" s="26"/>
     </row>
-    <row r="29" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="23" t="s">
         <v>95</v>
       </c>
@@ -2275,7 +2279,7 @@
       <c r="X29" s="26"/>
       <c r="Y29" s="26"/>
     </row>
-    <row r="30" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="40" t="s">
         <v>93</v>
       </c>
@@ -2310,8 +2314,8 @@
       <c r="X30" s="26"/>
       <c r="Y30" s="26"/>
     </row>
-    <row r="31" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="32" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A30:M30"/>
@@ -2324,6 +2328,9 @@
       <formula1>"Stock Part,Stock Material,Custom Part,Other"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="L4" r:id="rId1" xr:uid="{7F44BF34-D782-2D49-8653-933D5279BEC6}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>